<commit_message>
adding notes to abstract for paper
</commit_message>
<xml_diff>
--- a/OEB 53/papers/Evo.LitReview.xlsx
+++ b/OEB 53/papers/Evo.LitReview.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/classes/OEB 53/refs/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27729"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2700" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14320" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -17,20 +12,20 @@
     <sheet name="papers" sheetId="3" r:id="rId3"/>
     <sheet name="scratch" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="78">
   <si>
     <t>Literature Review for OEB 53 paper</t>
   </si>
@@ -284,19 +279,15 @@
   <si>
     <t>freezing tolerance diverged multiple times across oak tropical to temperate divide</t>
   </si>
+  <si>
+    <t>climatic stress and changes in climate result in selection of resistent genotypes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -341,7 +332,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,7 +390,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -434,7 +425,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -611,7 +602,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -625,39 +616,39 @@
       <selection activeCell="A15" sqref="A15:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1">
         <v>42824</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -665,7 +656,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -673,7 +664,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -681,53 +672,58 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1">
       <c r="A22" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -739,12 +735,12 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -758,7 +754,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>42824</v>
       </c>
@@ -772,7 +768,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>42824</v>
       </c>
@@ -786,7 +782,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>42824</v>
       </c>
@@ -802,6 +798,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -810,12 +811,12 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -841,7 +842,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -867,7 +868,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -893,7 +894,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -913,7 +914,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -933,7 +934,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -950,7 +951,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -967,7 +968,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -984,7 +985,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -1001,7 +1002,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -1018,7 +1019,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -1034,8 +1035,11 @@
       <c r="F11" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>73</v>
       </c>
@@ -1054,6 +1058,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1063,8 +1072,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>